<commit_message>
Change nain.py to new loop for
</commit_message>
<xml_diff>
--- a/parsing_settings.xlsx
+++ b/parsing_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\price-collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BECAF4-E6DE-4739-9501-00D5010DD3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A760220F-2001-4110-B22B-50EFA02997BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{A60456A8-5F9C-4F7F-8F96-122E924FA372}"/>
   </bookViews>
@@ -569,7 +569,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -814,7 +814,7 @@
         <v>19</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1308,7 +1308,7 @@
         <v>39</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add insert city, shop into varus_parser. Add utility to save to file
</commit_message>
<xml_diff>
--- a/parsing_settings.xlsx
+++ b/parsing_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\price-collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A760220F-2001-4110-B22B-50EFA02997BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD21F777-6510-4573-A839-3D831746BB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{A60456A8-5F9C-4F7F-8F96-122E924FA372}"/>
   </bookViews>
@@ -569,7 +569,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -814,7 +814,7 @@
         <v>19</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Merge devMTD with main
</commit_message>
<xml_diff>
--- a/parsing_settings.xlsx
+++ b/parsing_settings.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\price-collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A760220F-2001-4110-B22B-50EFA02997BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{A60456A8-5F9C-4F7F-8F96-122E924FA372}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15495"/>
   </bookViews>
   <sheets>
     <sheet name="parsing_settings_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -170,8 +169,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +215,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -233,17 +232,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4EA28B1-D4E7-4AD3-999E-4CA9A581BDE2}" name="Table1" displayName="Table1" ref="A1:H28" totalsRowShown="0">
-  <autoFilter ref="A1:H28" xr:uid="{C4EA28B1-D4E7-4AD3-999E-4CA9A581BDE2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H28" totalsRowShown="0">
+  <autoFilter ref="A1:H28"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{932CE544-B6C8-42D7-8967-24385E965613}" name="net_name"/>
-    <tableColumn id="2" xr3:uid="{AC54E5A5-301D-4778-9871-2094194A09A6}" name="url" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{AEBA268A-E09D-4D2B-AF5A-CE0938370AFD}" name="category_name"/>
-    <tableColumn id="4" xr3:uid="{751BD779-C01D-4206-B9BC-95B749F31273}" name="category_url" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{56F78AAA-82C6-45F2-9923-44E2FC4A21D5}" name="parser"/>
-    <tableColumn id="6" xr3:uid="{027074A0-363F-4EAB-A39E-3FAD23AB080F}" name="city_name"/>
-    <tableColumn id="7" xr3:uid="{106A54D0-70A0-4322-9F26-56E7F43D8609}" name="shop_address"/>
-    <tableColumn id="8" xr3:uid="{19ACFF51-B657-4BAF-8024-B634550B6945}" name="ToParse"/>
+    <tableColumn id="1" name="net_name"/>
+    <tableColumn id="2" name="url"/>
+    <tableColumn id="3" name="category_name"/>
+    <tableColumn id="4" name="category_url"/>
+    <tableColumn id="5" name="parser"/>
+    <tableColumn id="6" name="city_name"/>
+    <tableColumn id="7" name="shop_address"/>
+    <tableColumn id="8" name="ToParse"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -565,25 +564,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5676DB30-6FA6-4227-82A9-4C41CD017917}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +608,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -635,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -661,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -687,7 +686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -713,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -739,7 +738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -765,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -791,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -817,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -843,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -869,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -895,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -921,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -947,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -973,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -999,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1100,10 +1099,10 @@
         <v>30</v>
       </c>
       <c r="H20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1125,11 +1124,8 @@
       <c r="G21" t="s">
         <v>31</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1155,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1181,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1204,10 +1200,10 @@
         <v>35</v>
       </c>
       <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1233,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1259,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1282,10 +1278,10 @@
         <v>38</v>
       </c>
       <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1313,48 +1309,48 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H28" xr:uid="{7E58EC03-AE10-4613-8BC2-7DFF9B26160B}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H28">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{913F5F36-F395-4507-8086-F3EC87AEC8D9}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{0BA0E62D-CBE6-4635-8ECD-EBF6B1948357}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{728AA4FE-B999-4B32-B69D-D0BFA2593A1D}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{582A741E-5B68-4C3D-966E-EF2EBAD92F54}"/>
-    <hyperlink ref="D3" r:id="rId5" xr:uid="{E313AE8F-8E44-4BF2-A66C-187189750099}"/>
-    <hyperlink ref="D4" r:id="rId6" xr:uid="{6DA7F2D9-3200-460D-B94D-F8765AA15CF9}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{0BE8F6A2-D7F9-4938-ADE1-6C0949227D2C}"/>
-    <hyperlink ref="B5" r:id="rId8" xr:uid="{5FBEDB2B-2704-4725-8EE2-0E2FE804800E}"/>
-    <hyperlink ref="B6" r:id="rId9" xr:uid="{5B004A94-6DAB-4AF0-B152-11045A65ECA2}"/>
-    <hyperlink ref="B7" r:id="rId10" xr:uid="{F474CDEB-E40E-4C8D-921C-F9F77814B346}"/>
-    <hyperlink ref="D6" r:id="rId11" xr:uid="{B81E1E80-EA39-4B4C-92EA-5F9AA8C0683F}"/>
-    <hyperlink ref="D7" r:id="rId12" xr:uid="{93FA332A-7266-4970-90A3-D1BA72066C8D}"/>
-    <hyperlink ref="B8" r:id="rId13" xr:uid="{EE0B4F26-DDE5-4DDB-9DA3-941D225B2DAA}"/>
-    <hyperlink ref="D8" r:id="rId14" xr:uid="{152DFD36-6CB9-449B-B9B9-C423A84C56D3}"/>
-    <hyperlink ref="B9" r:id="rId15" xr:uid="{7D306C43-DA5B-480D-B08A-C3F2BF2581E0}"/>
-    <hyperlink ref="B10" r:id="rId16" xr:uid="{A693A107-2A82-4E23-B11C-2407BE69C641}"/>
-    <hyperlink ref="D9" r:id="rId17" xr:uid="{79DA5B01-5BD4-4FDA-BC52-1CB800D0D238}"/>
-    <hyperlink ref="D10" r:id="rId18" xr:uid="{6FA7495D-0B60-4E25-89C8-EC7B62CAF948}"/>
-    <hyperlink ref="D11" r:id="rId19" xr:uid="{E44437FA-9544-46E6-A4CB-787B99270ACF}"/>
-    <hyperlink ref="B11" r:id="rId20" xr:uid="{2DF3BCEF-AF1C-44C8-AD77-46586E0784C0}"/>
-    <hyperlink ref="B12" r:id="rId21" xr:uid="{346C6885-AF71-4C72-8497-9947A330F1E9}"/>
-    <hyperlink ref="B13" r:id="rId22" xr:uid="{7F1AA1A2-2FF6-41E7-AF0B-D1BFECA52910}"/>
-    <hyperlink ref="D12" r:id="rId23" xr:uid="{E031C327-2E8A-4189-BE24-47BDDC345001}"/>
-    <hyperlink ref="D13" r:id="rId24" xr:uid="{6B4EAECC-6F8E-4CAC-A8CD-9921D512F65D}"/>
-    <hyperlink ref="B14" r:id="rId25" xr:uid="{4737DA1F-4A6B-46BF-9FB7-179A3C9BF2D6}"/>
-    <hyperlink ref="D14" r:id="rId26" xr:uid="{0A7561D7-A9D0-448A-8D02-0CF9D655E92B}"/>
-    <hyperlink ref="B15" r:id="rId27" xr:uid="{FA2E0783-F902-4324-AA91-8887289C4FB9}"/>
-    <hyperlink ref="B16" r:id="rId28" xr:uid="{850B891C-5E57-4547-A489-33A47C9C0C41}"/>
-    <hyperlink ref="D15" r:id="rId29" xr:uid="{12D7FFCF-29D2-4738-BBD2-24FC96FABF55}"/>
-    <hyperlink ref="D16" r:id="rId30" xr:uid="{DEA5589E-6C50-413D-B6EC-EDCBC48FAAD2}"/>
-    <hyperlink ref="D17" r:id="rId31" xr:uid="{D12AC4FB-0107-4FCD-ABAA-44E38ABE3F56}"/>
-    <hyperlink ref="B17" r:id="rId32" xr:uid="{6E71AE1D-C562-47AC-9536-7ADF86447967}"/>
-    <hyperlink ref="B18" r:id="rId33" xr:uid="{967E17DC-EE01-4C3C-9F78-CD8ECE76DA7E}"/>
-    <hyperlink ref="B19" r:id="rId34" xr:uid="{677B05F6-A550-44A5-B861-D4BC0212F48D}"/>
-    <hyperlink ref="D18" r:id="rId35" xr:uid="{D7F0C174-921A-4DD3-A6B3-AADA3DAA4F47}"/>
-    <hyperlink ref="D19" r:id="rId36" xr:uid="{E6E3B420-D7A2-41F9-9115-389BE8792257}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="D3" r:id="rId5"/>
+    <hyperlink ref="D4" r:id="rId6"/>
+    <hyperlink ref="D5" r:id="rId7"/>
+    <hyperlink ref="B5" r:id="rId8"/>
+    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="B7" r:id="rId10"/>
+    <hyperlink ref="D6" r:id="rId11"/>
+    <hyperlink ref="D7" r:id="rId12"/>
+    <hyperlink ref="B8" r:id="rId13"/>
+    <hyperlink ref="D8" r:id="rId14"/>
+    <hyperlink ref="B9" r:id="rId15"/>
+    <hyperlink ref="B10" r:id="rId16"/>
+    <hyperlink ref="D9" r:id="rId17"/>
+    <hyperlink ref="D10" r:id="rId18"/>
+    <hyperlink ref="D11" r:id="rId19"/>
+    <hyperlink ref="B11" r:id="rId20"/>
+    <hyperlink ref="B12" r:id="rId21"/>
+    <hyperlink ref="B13" r:id="rId22"/>
+    <hyperlink ref="D12" r:id="rId23"/>
+    <hyperlink ref="D13" r:id="rId24"/>
+    <hyperlink ref="B14" r:id="rId25"/>
+    <hyperlink ref="D14" r:id="rId26"/>
+    <hyperlink ref="B15" r:id="rId27"/>
+    <hyperlink ref="B16" r:id="rId28"/>
+    <hyperlink ref="D15" r:id="rId29"/>
+    <hyperlink ref="D16" r:id="rId30"/>
+    <hyperlink ref="D17" r:id="rId31"/>
+    <hyperlink ref="B17" r:id="rId32"/>
+    <hyperlink ref="B18" r:id="rId33"/>
+    <hyperlink ref="B19" r:id="rId34"/>
+    <hyperlink ref="D18" r:id="rId35"/>
+    <hyperlink ref="D19" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
done silpo + spec files
</commit_message>
<xml_diff>
--- a/parsing_settings.xlsx
+++ b/parsing_settings.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="44">
   <si>
     <t>net_name</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>ToParse</t>
+  </si>
+  <si>
+    <t>Бровари</t>
+  </si>
+  <si>
+    <t>вул. Київська, 156</t>
   </si>
 </sst>
 </file>
@@ -232,8 +238,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H28" totalsRowShown="0">
-  <autoFilter ref="A1:H28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H29" totalsRowShown="0">
+  <autoFilter ref="A1:H29"/>
   <tableColumns count="8">
     <tableColumn id="1" name="net_name"/>
     <tableColumn id="2" name="url"/>
@@ -565,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -631,7 +637,7 @@
         <v>12</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -683,7 +689,7 @@
         <v>14</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -813,7 +819,7 @@
         <v>19</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -839,7 +845,7 @@
         <v>20</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -969,7 +975,7 @@
         <v>23</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1099,7 +1105,7 @@
         <v>30</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1124,6 +1130,9 @@
       <c r="G21" t="s">
         <v>31</v>
       </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
@@ -1200,7 +1209,7 @@
         <v>35</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1226,7 +1235,7 @@
         <v>36</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1307,9 +1316,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H28">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H29">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>